<commit_message>
3.0.3: Support alias and aliasTs for toJSON.
</commit_message>
<xml_diff>
--- a/meta/program/BlancoValueObjectTsFieldStructure.xlsx
+++ b/meta/program/BlancoValueObjectTsFieldStructure.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoValueObjectTs/meta/program/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{835CBDF3-3E42-3B47-80C2-B8796B9F3A89}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF797CC7-3AC4-F64F-853C-2307353C1A4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="460" windowWidth="28300" windowHeight="17440" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4780" yWindow="7640" windowWidth="28300" windowHeight="17440" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="valueObject" sheetId="1" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="79">
   <si>
     <t>バリューオブジェクト定義書</t>
   </si>
@@ -400,6 +400,23 @@
     </rPh>
     <rPh sb="12" eb="14">
       <t xml:space="preserve">バアイハ </t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>alias</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>フィールド名の別名を指定します。toJSONに反映されます。</t>
+    <rPh sb="7" eb="9">
+      <t xml:space="preserve">ベツメイヲ </t>
+    </rPh>
+    <rPh sb="10" eb="12">
+      <t xml:space="preserve">シテイシマス。 </t>
+    </rPh>
+    <rPh sb="23" eb="25">
+      <t xml:space="preserve">ハンエイ </t>
     </rPh>
     <phoneticPr fontId="3"/>
   </si>
@@ -798,16 +815,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -898,7 +914,6 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -929,10 +944,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -941,7 +956,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1354,10 +1369,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G49"/>
+  <dimension ref="A1:G50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -1374,7 +1389,7 @@
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="29" t="s">
+      <c r="F1" s="28" t="s">
         <v>29</v>
       </c>
       <c r="G1"/>
@@ -1404,50 +1419,50 @@
       <c r="G5"/>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="17" t="s">
+      <c r="A6" s="16" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="6"/>
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="D6" s="11"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="13"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="12"/>
       <c r="G6"/>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="17" t="s">
+      <c r="A7" s="16" t="s">
         <v>5</v>
       </c>
       <c r="B7" s="6"/>
-      <c r="C7" s="14" t="s">
+      <c r="C7" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="D7" s="15"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="13"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="12"/>
       <c r="G7"/>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" s="17" t="s">
+      <c r="A8" s="16" t="s">
         <v>12</v>
       </c>
       <c r="B8" s="6"/>
-      <c r="C8" s="10" t="s">
+      <c r="C8" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="D8" s="16"/>
-      <c r="E8" s="16"/>
-      <c r="F8" s="11"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="10"/>
       <c r="G8"/>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="17" t="s">
+      <c r="A9" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="B9" s="8"/>
-      <c r="C9" s="33" t="s">
+      <c r="B9" s="7"/>
+      <c r="C9" s="32" t="s">
         <v>27</v>
       </c>
       <c r="D9"/>
@@ -1456,22 +1471,22 @@
       <c r="G9"/>
     </row>
     <row r="10" spans="1:7">
-      <c r="A10" s="17" t="s">
+      <c r="A10" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="B10" s="8"/>
-      <c r="C10" s="33"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="32"/>
       <c r="D10"/>
       <c r="E10"/>
       <c r="F10"/>
       <c r="G10"/>
     </row>
     <row r="11" spans="1:7">
-      <c r="A11" s="17" t="s">
+      <c r="A11" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="8"/>
-      <c r="C11" s="33" t="s">
+      <c r="B11" s="7"/>
+      <c r="C11" s="32" t="s">
         <v>17</v>
       </c>
       <c r="D11"/>
@@ -1480,11 +1495,11 @@
       <c r="G11"/>
     </row>
     <row r="12" spans="1:7">
-      <c r="A12" s="17" t="s">
+      <c r="A12" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="8"/>
-      <c r="C12" s="33" t="s">
+      <c r="B12" s="7"/>
+      <c r="C12" s="32" t="s">
         <v>17</v>
       </c>
       <c r="D12"/>
@@ -1493,22 +1508,22 @@
       <c r="G12"/>
     </row>
     <row r="13" spans="1:7">
-      <c r="A13" s="17" t="s">
+      <c r="A13" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="8"/>
-      <c r="C13" s="33"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="32"/>
       <c r="D13"/>
       <c r="E13"/>
       <c r="F13"/>
       <c r="G13"/>
     </row>
     <row r="14" spans="1:7">
-      <c r="A14" s="7"/>
-      <c r="B14" s="7"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
+      <c r="A14"/>
+      <c r="B14"/>
+      <c r="C14"/>
+      <c r="D14"/>
+      <c r="E14"/>
       <c r="G14"/>
     </row>
     <row r="15" spans="1:7">
@@ -1522,486 +1537,501 @@
       <c r="G15"/>
     </row>
     <row r="16" spans="1:7">
-      <c r="A16" s="17" t="s">
+      <c r="A16" s="16" t="s">
         <v>4</v>
       </c>
       <c r="B16" s="6"/>
-      <c r="C16" s="10"/>
-      <c r="D16" s="16"/>
-      <c r="E16" s="11"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="15"/>
+      <c r="E16" s="10"/>
       <c r="G16"/>
     </row>
     <row r="17" spans="1:7">
-      <c r="A17" s="7"/>
-      <c r="B17" s="7"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="39"/>
-      <c r="E17" s="39"/>
+      <c r="A17"/>
+      <c r="B17"/>
+      <c r="C17"/>
+      <c r="D17"/>
+      <c r="E17"/>
       <c r="G17"/>
     </row>
     <row r="18" spans="1:7">
       <c r="A18" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B18" s="8"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="8"/>
+      <c r="B18" s="7"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
       <c r="E18" s="6"/>
       <c r="F18"/>
       <c r="G18"/>
     </row>
     <row r="19" spans="1:7">
-      <c r="A19" s="52" t="s">
+      <c r="A19" s="50" t="s">
         <v>7</v>
       </c>
-      <c r="B19" s="53" t="s">
+      <c r="B19" s="51" t="s">
         <v>11</v>
       </c>
-      <c r="C19" s="54"/>
-      <c r="D19" s="54"/>
-      <c r="E19" s="50"/>
+      <c r="C19" s="52"/>
+      <c r="D19" s="52"/>
+      <c r="E19" s="48"/>
       <c r="F19"/>
       <c r="G19"/>
     </row>
     <row r="20" spans="1:7">
-      <c r="A20" s="52"/>
-      <c r="B20" s="53"/>
-      <c r="C20" s="54"/>
-      <c r="D20" s="54"/>
-      <c r="E20" s="50"/>
+      <c r="A20" s="50"/>
+      <c r="B20" s="51"/>
+      <c r="C20" s="52"/>
+      <c r="D20" s="52"/>
+      <c r="E20" s="48"/>
       <c r="F20"/>
       <c r="G20"/>
     </row>
     <row r="21" spans="1:7">
-      <c r="A21" s="18"/>
-      <c r="B21" s="20"/>
-      <c r="C21" s="27"/>
-      <c r="D21" s="27"/>
-      <c r="E21" s="37"/>
+      <c r="A21" s="17"/>
+      <c r="B21" s="19"/>
+      <c r="C21" s="26"/>
+      <c r="D21" s="26"/>
+      <c r="E21" s="36"/>
       <c r="F21"/>
       <c r="G21"/>
     </row>
     <row r="22" spans="1:7">
-      <c r="A22" s="22"/>
-      <c r="B22" s="24"/>
-      <c r="C22" s="28"/>
-      <c r="D22" s="28"/>
-      <c r="E22" s="38"/>
+      <c r="A22" s="21"/>
+      <c r="B22" s="23"/>
+      <c r="C22" s="27"/>
+      <c r="D22" s="27"/>
+      <c r="E22" s="37"/>
       <c r="F22"/>
       <c r="G22"/>
     </row>
     <row r="23" spans="1:7">
-      <c r="A23" s="7"/>
-      <c r="B23" s="7"/>
-      <c r="C23" s="7"/>
-      <c r="D23" s="7"/>
-      <c r="E23" s="7"/>
+      <c r="A23"/>
+      <c r="B23"/>
+      <c r="C23"/>
+      <c r="D23"/>
+      <c r="E23"/>
       <c r="G23"/>
     </row>
     <row r="24" spans="1:7">
       <c r="A24" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B24" s="8"/>
-      <c r="C24" s="8"/>
-      <c r="D24" s="8"/>
-      <c r="E24" s="8"/>
+      <c r="B24" s="7"/>
+      <c r="C24" s="7"/>
+      <c r="D24" s="7"/>
+      <c r="E24" s="7"/>
       <c r="F24" s="6"/>
       <c r="G24"/>
     </row>
     <row r="25" spans="1:7" ht="13.5" customHeight="1">
-      <c r="A25" s="52" t="s">
+      <c r="A25" s="50" t="s">
         <v>7</v>
       </c>
-      <c r="B25" s="52" t="s">
+      <c r="B25" s="50" t="s">
         <v>8</v>
       </c>
-      <c r="C25" s="51" t="s">
+      <c r="C25" s="49" t="s">
         <v>9</v>
       </c>
-      <c r="D25" s="51" t="s">
+      <c r="D25" s="49" t="s">
         <v>10</v>
       </c>
-      <c r="E25" s="51" t="s">
+      <c r="E25" s="49" t="s">
         <v>6</v>
       </c>
-      <c r="F25" s="26"/>
+      <c r="F25" s="25"/>
       <c r="G25"/>
     </row>
     <row r="26" spans="1:7">
-      <c r="A26" s="52"/>
-      <c r="B26" s="52"/>
-      <c r="C26" s="51"/>
-      <c r="D26" s="51"/>
-      <c r="E26" s="51"/>
-      <c r="F26" s="9"/>
+      <c r="A26" s="50"/>
+      <c r="B26" s="50"/>
+      <c r="C26" s="49"/>
+      <c r="D26" s="49"/>
+      <c r="E26" s="49"/>
+      <c r="F26" s="8"/>
       <c r="G26"/>
     </row>
     <row r="27" spans="1:7">
-      <c r="A27" s="18">
+      <c r="A27" s="17">
         <v>1</v>
       </c>
-      <c r="B27" s="19" t="s">
+      <c r="B27" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="C27" s="20" t="s">
+      <c r="C27" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="D27" s="20"/>
-      <c r="E27" s="20" t="s">
+      <c r="D27" s="19"/>
+      <c r="E27" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="F27" s="21"/>
+      <c r="F27" s="20"/>
       <c r="G27"/>
     </row>
     <row r="28" spans="1:7">
-      <c r="A28" s="40">
+      <c r="A28" s="38">
         <f>A27+1</f>
         <v>2</v>
       </c>
-      <c r="B28" s="41" t="s">
+      <c r="B28" s="39" t="s">
         <v>35</v>
       </c>
-      <c r="C28" s="42" t="s">
+      <c r="C28" s="40" t="s">
         <v>33</v>
       </c>
-      <c r="D28" s="42"/>
-      <c r="E28" s="42" t="s">
+      <c r="D28" s="40"/>
+      <c r="E28" s="40" t="s">
         <v>36</v>
       </c>
-      <c r="F28" s="43"/>
+      <c r="F28" s="41"/>
       <c r="G28"/>
     </row>
     <row r="29" spans="1:7">
-      <c r="A29" s="40">
-        <f t="shared" ref="A29:A45" si="0">A28+1</f>
+      <c r="A29" s="38">
+        <f>A27+1</f>
+        <v>2</v>
+      </c>
+      <c r="B29" s="39" t="s">
+        <v>77</v>
+      </c>
+      <c r="C29" s="40" t="s">
+        <v>33</v>
+      </c>
+      <c r="D29" s="40"/>
+      <c r="E29" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="F29" s="41"/>
+      <c r="G29"/>
+    </row>
+    <row r="30" spans="1:7">
+      <c r="A30" s="38">
+        <f>A28+1</f>
         <v>3</v>
       </c>
-      <c r="B29" s="41" t="s">
+      <c r="B30" s="39" t="s">
         <v>37</v>
       </c>
-      <c r="C29" s="42" t="s">
+      <c r="C30" s="40" t="s">
         <v>33</v>
       </c>
-      <c r="D29" s="42"/>
-      <c r="E29" s="42" t="s">
+      <c r="D30" s="40"/>
+      <c r="E30" s="40" t="s">
         <v>38</v>
       </c>
-      <c r="F29" s="43"/>
-      <c r="G29"/>
-    </row>
-    <row r="30" spans="1:7">
-      <c r="A30" s="40">
-        <f t="shared" si="0"/>
+      <c r="F30" s="41"/>
+      <c r="G30"/>
+    </row>
+    <row r="31" spans="1:7">
+      <c r="A31" s="38">
+        <f t="shared" ref="A31:A46" si="0">A30+1</f>
         <v>4</v>
       </c>
-      <c r="B30" s="41" t="s">
+      <c r="B31" s="39" t="s">
         <v>59</v>
       </c>
-      <c r="C30" s="42" t="s">
+      <c r="C31" s="40" t="s">
         <v>33</v>
       </c>
-      <c r="D30" s="42"/>
-      <c r="E30" s="42" t="s">
+      <c r="D31" s="40"/>
+      <c r="E31" s="40" t="s">
         <v>60</v>
       </c>
-      <c r="F30" s="43"/>
-      <c r="G30"/>
-    </row>
-    <row r="31" spans="1:7" ht="45">
-      <c r="A31" s="40">
+      <c r="F31" s="41"/>
+      <c r="G31"/>
+    </row>
+    <row r="32" spans="1:7" ht="45">
+      <c r="A32" s="38">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="B31" s="44" t="s">
+      <c r="B32" s="42" t="s">
         <v>62</v>
       </c>
-      <c r="C31" s="45" t="s">
+      <c r="C32" s="43" t="s">
         <v>55</v>
       </c>
-      <c r="D31" s="45" t="s">
+      <c r="D32" s="43" t="s">
         <v>56</v>
       </c>
-      <c r="E31" s="45" t="s">
+      <c r="E32" s="43" t="s">
         <v>61</v>
       </c>
-      <c r="F31" s="46"/>
-      <c r="G31"/>
-    </row>
-    <row r="32" spans="1:7">
-      <c r="A32" s="40">
+      <c r="F32" s="44"/>
+      <c r="G32"/>
+    </row>
+    <row r="33" spans="1:7">
+      <c r="A33" s="38">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="B32" s="41" t="s">
+      <c r="B33" s="39" t="s">
         <v>39</v>
       </c>
-      <c r="C32" s="42" t="s">
+      <c r="C33" s="40" t="s">
         <v>33</v>
       </c>
-      <c r="D32" s="42"/>
-      <c r="E32" s="42" t="s">
+      <c r="D33" s="40"/>
+      <c r="E33" s="40" t="s">
         <v>40</v>
       </c>
-      <c r="F32" s="43"/>
-      <c r="G32"/>
-    </row>
-    <row r="33" spans="1:7">
-      <c r="A33" s="40">
+      <c r="F33" s="41"/>
+      <c r="G33"/>
+    </row>
+    <row r="34" spans="1:7">
+      <c r="A34" s="38">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="B33" s="41" t="s">
+      <c r="B34" s="39" t="s">
         <v>71</v>
       </c>
-      <c r="C33" s="42" t="s">
+      <c r="C34" s="40" t="s">
         <v>64</v>
       </c>
-      <c r="D33" s="47" t="s">
+      <c r="D34" s="45" t="s">
         <v>65</v>
       </c>
-      <c r="E33" s="42" t="s">
+      <c r="E34" s="40" t="s">
         <v>72</v>
       </c>
-      <c r="F33" s="43"/>
-      <c r="G33"/>
-    </row>
-    <row r="34" spans="1:7">
-      <c r="A34" s="40">
+      <c r="F34" s="41"/>
+      <c r="G34"/>
+    </row>
+    <row r="35" spans="1:7">
+      <c r="A35" s="38">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="B34" s="41" t="s">
+      <c r="B35" s="39" t="s">
         <v>63</v>
       </c>
-      <c r="C34" s="42" t="s">
+      <c r="C35" s="40" t="s">
         <v>64</v>
       </c>
-      <c r="D34" s="47" t="s">
+      <c r="D35" s="45" t="s">
         <v>65</v>
       </c>
-      <c r="E34" s="42" t="s">
+      <c r="E35" s="40" t="s">
         <v>68</v>
       </c>
-      <c r="F34" s="43"/>
-      <c r="G34"/>
-    </row>
-    <row r="35" spans="1:7">
-      <c r="A35" s="40">
+      <c r="F35" s="41"/>
+      <c r="G35"/>
+    </row>
+    <row r="36" spans="1:7">
+      <c r="A36" s="38">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="B35" s="41" t="s">
+      <c r="B36" s="39" t="s">
         <v>66</v>
       </c>
-      <c r="C35" s="42" t="s">
+      <c r="C36" s="40" t="s">
         <v>64</v>
       </c>
-      <c r="D35" s="47" t="s">
+      <c r="D36" s="45" t="s">
         <v>65</v>
       </c>
-      <c r="E35" s="42" t="s">
+      <c r="E36" s="40" t="s">
         <v>69</v>
       </c>
-      <c r="F35" s="43"/>
-      <c r="G35"/>
-    </row>
-    <row r="36" spans="1:7">
-      <c r="A36" s="40">
+      <c r="F36" s="41"/>
+      <c r="G36"/>
+    </row>
+    <row r="37" spans="1:7">
+      <c r="A37" s="38">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="B36" s="41" t="s">
+      <c r="B37" s="39" t="s">
         <v>67</v>
       </c>
-      <c r="C36" s="42" t="s">
+      <c r="C37" s="40" t="s">
         <v>64</v>
       </c>
-      <c r="D36" s="47" t="s">
+      <c r="D37" s="45" t="s">
         <v>65</v>
       </c>
-      <c r="E36" s="42" t="s">
+      <c r="E37" s="40" t="s">
         <v>70</v>
       </c>
-      <c r="F36" s="43"/>
-      <c r="G36"/>
-    </row>
-    <row r="37" spans="1:7">
-      <c r="A37" s="40">
+      <c r="F37" s="41"/>
+      <c r="G37"/>
+    </row>
+    <row r="38" spans="1:7">
+      <c r="A38" s="38">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="B37" s="41" t="s">
+      <c r="B38" s="39" t="s">
         <v>75</v>
       </c>
-      <c r="C37" s="42" t="s">
+      <c r="C38" s="40" t="s">
         <v>64</v>
       </c>
-      <c r="D37" s="47" t="s">
+      <c r="D38" s="45" t="s">
         <v>65</v>
       </c>
-      <c r="E37" s="42" t="s">
+      <c r="E38" s="40" t="s">
         <v>76</v>
       </c>
-      <c r="F37" s="43"/>
-      <c r="G37"/>
-    </row>
-    <row r="38" spans="1:7">
-      <c r="A38" s="40">
+      <c r="F38" s="41"/>
+      <c r="G38"/>
+    </row>
+    <row r="39" spans="1:7">
+      <c r="A39" s="38">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="B38" s="41" t="s">
+      <c r="B39" s="39" t="s">
         <v>41</v>
       </c>
-      <c r="C38" s="42" t="s">
+      <c r="C39" s="40" t="s">
         <v>33</v>
       </c>
-      <c r="D38" s="42"/>
-      <c r="E38" s="42" t="s">
+      <c r="D39" s="40"/>
+      <c r="E39" s="40" t="s">
         <v>57</v>
       </c>
-      <c r="F38" s="43"/>
-      <c r="G38"/>
-    </row>
-    <row r="39" spans="1:7" ht="45">
-      <c r="A39" s="40">
+      <c r="F39" s="41"/>
+      <c r="G39"/>
+    </row>
+    <row r="40" spans="1:7" ht="45">
+      <c r="A40" s="38">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="B39" s="44" t="s">
+      <c r="B40" s="42" t="s">
         <v>54</v>
       </c>
-      <c r="C39" s="45" t="s">
+      <c r="C40" s="43" t="s">
         <v>55</v>
       </c>
-      <c r="D39" s="45" t="s">
+      <c r="D40" s="43" t="s">
         <v>56</v>
       </c>
-      <c r="E39" s="48" t="s">
+      <c r="E40" s="46" t="s">
         <v>58</v>
       </c>
-      <c r="F39" s="49"/>
-      <c r="G39"/>
-    </row>
-    <row r="40" spans="1:7">
-      <c r="A40" s="40">
+      <c r="F40" s="47"/>
+      <c r="G40"/>
+    </row>
+    <row r="41" spans="1:7">
+      <c r="A41" s="38">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="B40" s="41" t="s">
+      <c r="B41" s="39" t="s">
         <v>42</v>
       </c>
-      <c r="C40" s="42" t="s">
+      <c r="C41" s="40" t="s">
         <v>33</v>
       </c>
-      <c r="D40" s="42"/>
-      <c r="E40" s="42" t="s">
+      <c r="D41" s="40"/>
+      <c r="E41" s="40" t="s">
         <v>43</v>
       </c>
-      <c r="F40" s="43"/>
-      <c r="G40"/>
-    </row>
-    <row r="41" spans="1:7">
-      <c r="A41" s="40">
+      <c r="F41" s="41"/>
+      <c r="G41"/>
+    </row>
+    <row r="42" spans="1:7">
+      <c r="A42" s="38">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="B41" s="41" t="s">
+      <c r="B42" s="39" t="s">
         <v>44</v>
       </c>
-      <c r="C41" s="42" t="s">
+      <c r="C42" s="40" t="s">
         <v>33</v>
       </c>
-      <c r="D41" s="42"/>
-      <c r="E41" s="42" t="s">
+      <c r="D42" s="40"/>
+      <c r="E42" s="40" t="s">
         <v>45</v>
       </c>
-      <c r="F41" s="43"/>
-      <c r="G41"/>
-    </row>
-    <row r="42" spans="1:7">
-      <c r="A42" s="40">
+      <c r="F42" s="41"/>
+      <c r="G42"/>
+    </row>
+    <row r="43" spans="1:7">
+      <c r="A43" s="38">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="B42" s="41" t="s">
+      <c r="B43" s="39" t="s">
         <v>46</v>
       </c>
-      <c r="C42" s="42" t="s">
+      <c r="C43" s="40" t="s">
         <v>33</v>
       </c>
-      <c r="D42" s="42"/>
-      <c r="E42" s="42" t="s">
+      <c r="D43" s="40"/>
+      <c r="E43" s="40" t="s">
         <v>47</v>
       </c>
-      <c r="F42" s="43"/>
-      <c r="G42"/>
-    </row>
-    <row r="43" spans="1:7">
-      <c r="A43" s="40">
+      <c r="F43" s="41"/>
+      <c r="G43"/>
+    </row>
+    <row r="44" spans="1:7">
+      <c r="A44" s="38">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="B43" s="41" t="s">
+      <c r="B44" s="39" t="s">
         <v>48</v>
       </c>
-      <c r="C43" s="42" t="s">
+      <c r="C44" s="40" t="s">
         <v>33</v>
       </c>
-      <c r="D43" s="42"/>
-      <c r="E43" s="42" t="s">
+      <c r="D44" s="40"/>
+      <c r="E44" s="40" t="s">
         <v>49</v>
       </c>
-      <c r="F43" s="43"/>
-      <c r="G43"/>
-    </row>
-    <row r="44" spans="1:7">
-      <c r="A44" s="40">
+      <c r="F44" s="41"/>
+      <c r="G44"/>
+    </row>
+    <row r="45" spans="1:7">
+      <c r="A45" s="38">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="B44" s="41" t="s">
+      <c r="B45" s="39" t="s">
         <v>50</v>
       </c>
-      <c r="C44" s="42" t="s">
+      <c r="C45" s="40" t="s">
         <v>33</v>
       </c>
-      <c r="D44" s="42"/>
-      <c r="E44" s="42" t="s">
+      <c r="D45" s="40"/>
+      <c r="E45" s="40" t="s">
         <v>51</v>
       </c>
-      <c r="F44" s="43"/>
-      <c r="G44"/>
-    </row>
-    <row r="45" spans="1:7">
-      <c r="A45" s="40">
+      <c r="F45" s="41"/>
+      <c r="G45"/>
+    </row>
+    <row r="46" spans="1:7">
+      <c r="A46" s="38">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="B45" s="41" t="s">
+      <c r="B46" s="39" t="s">
         <v>52</v>
       </c>
-      <c r="C45" s="42" t="s">
+      <c r="C46" s="40" t="s">
         <v>33</v>
       </c>
-      <c r="D45" s="42"/>
-      <c r="E45" s="42" t="s">
+      <c r="D46" s="40"/>
+      <c r="E46" s="40" t="s">
         <v>53</v>
       </c>
-      <c r="F45" s="43"/>
-      <c r="G45"/>
-    </row>
-    <row r="46" spans="1:7">
-      <c r="A46" s="22"/>
-      <c r="B46" s="23"/>
-      <c r="C46" s="24"/>
-      <c r="D46" s="24"/>
-      <c r="E46" s="24"/>
-      <c r="F46" s="25"/>
+      <c r="F46" s="41"/>
       <c r="G46"/>
     </row>
     <row r="47" spans="1:7">
+      <c r="A47" s="21"/>
+      <c r="B47" s="22"/>
+      <c r="C47" s="23"/>
+      <c r="D47" s="23"/>
+      <c r="E47" s="23"/>
+      <c r="F47" s="24"/>
       <c r="G47"/>
     </row>
     <row r="48" spans="1:7">
@@ -2010,9 +2040,12 @@
     <row r="49" spans="7:7">
       <c r="G49"/>
     </row>
+    <row r="50" spans="7:7">
+      <c r="G50"/>
+    </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="E39:F39"/>
+    <mergeCell ref="E40:F40"/>
     <mergeCell ref="E19:E20"/>
     <mergeCell ref="E25:E26"/>
     <mergeCell ref="A25:A26"/>
@@ -2026,7 +2059,7 @@
   </mergeCells>
   <phoneticPr fontId="3"/>
   <dataValidations count="6">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D62" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D63" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>型</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -2085,54 +2118,54 @@
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
-      <c r="J1" s="29" t="s">
+      <c r="J1" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="M1" s="29"/>
+      <c r="M1" s="28"/>
     </row>
     <row r="3" spans="1:13">
-      <c r="B3" s="32" t="s">
+      <c r="B3" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="D3" s="32" t="s">
+      <c r="D3" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="F3" s="32" t="s">
+      <c r="F3" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="H3" s="32" t="s">
+      <c r="H3" s="31" t="s">
         <v>19</v>
       </c>
-      <c r="J3" s="32" t="s">
+      <c r="J3" s="31" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:13">
-      <c r="B4" s="34"/>
-      <c r="D4" s="30"/>
-      <c r="F4" s="30"/>
-      <c r="H4" s="30"/>
-      <c r="J4" s="30"/>
+      <c r="B4" s="33"/>
+      <c r="D4" s="29"/>
+      <c r="F4" s="29"/>
+      <c r="H4" s="29"/>
+      <c r="J4" s="29"/>
     </row>
     <row r="5" spans="1:13">
-      <c r="B5" s="35" t="s">
+      <c r="B5" s="34" t="s">
         <v>28</v>
       </c>
-      <c r="D5" s="31" t="s">
+      <c r="D5" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="F5" s="31" t="s">
+      <c r="F5" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="H5" s="31" t="s">
+      <c r="H5" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="J5" s="31" t="s">
+      <c r="J5" s="30" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:13">
-      <c r="B6" s="36"/>
+      <c r="B6" s="35"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3"/>

</xml_diff>